<commit_message>
Added Cucumber framework and testNG framework
</commit_message>
<xml_diff>
--- a/src/test/resources/MiniProject.xlsx
+++ b/src/test/resources/MiniProject.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="8">
   <si>
     <t>User Name</t>
   </si>
@@ -111,11 +111,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
@@ -434,10 +436,10 @@
       <c r="B2" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s" s="5">
+      <c r="D2" t="s" s="7">
         <v>6</v>
       </c>
     </row>

</xml_diff>